<commit_message>
Update & add more files of competitive audit & report
</commit_message>
<xml_diff>
--- a/02-ux-design-process/Week4: Ideation/Competitive-audit/Activity/Competitive-audit-CoffeeHouse.xlsx
+++ b/02-ux-design-process/Week4: Ideation/Competitive-audit/Activity/Competitive-audit-CoffeeHouse.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t xml:space="preserve">Competitive audit
 </t>
@@ -245,6 +245,664 @@
   </si>
   <si>
     <t xml:space="preserve">Highest quality ingredients</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Outstanding
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Website is well designed and easy to use
++ Elegant design with strong branding</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Outstanding
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Website is highly responsive.
++Smooth ordering process. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Online ordering feature
++ User sign up feature</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Website available in two languages
+- Menu isn’t compatible with screen reader technologies</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Easy to find key info
+- No clear hierarchy, difficult to scan quickly</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Outstanding
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Easy to navigate
++ Clear indication of clickable elements</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Clear color scheme, font , and art direction
+- Inconsistent use of imagery and photography </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Serious and direct. Friendly in some places. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Outstanding
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ All key info is present
++ Short and to the point</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortitude Coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">York Place, Edinburgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 coffee flavours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$8 - $20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fortitudecoffee.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specialty coffee</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Modern minimalist design
+- Limited features available in desktop version. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Design is clean and easy to use
+- Some features don’t work as intended.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Outstanding
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Create account feature
++ Store locator feature. Online ordering feature with pickup/delivery options.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Outstanding
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Website available in six languages
++ Menu is compatible with screen reader technologies.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Easy to find menu
+- Home page is cluttered with many images</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Outstanding
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Very easy to navigate
++ Familiar way to navigate e.g., swipe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RATING
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Strong brand identity, including colors, fonts, style, motion, imagery, and photography</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Friendly and indirect</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Okay
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ All key info is present
+- Unnecessary details</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Green Leaf Cafe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indirect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whitechapel Rd, London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hot beverages, Coffee, Paan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$5 - $20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cafegreenleaf.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesmerizing taste &amp; aroma</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Need work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Manageable design
+- Missing footer and broken links. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Need work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Not fully responsive
+- Key information not available</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Needs work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- No checkout feature
+- Menus are only available through PDF downloads</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Needs work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Images of menus are not visible
+- Website only available in English</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Needs work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Home page is informative
+- Other pages are not functioning</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Needs work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Difficult to navigate due to big animation size
+- Some elements seem clickable but are not</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Needs work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- No brand identity at all</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Fun and indirect</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Needs work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Unnecessary details
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Too descriptive</t>
+    </r>
   </si>
   <si>
     <r>
@@ -272,6 +930,31 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Okay
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Easy to switch locations and languages
+- Somewhat difficult to navigate </t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Brief description </t>
   </si>
   <si>
@@ -298,48 +981,6 @@
       <t xml:space="preserve">+ Successes
 - Drawbacks</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Fortitude Coffee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">York Place, Edinburgh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 coffee flavours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$8 - $20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fortitudecoffee.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specialty coffee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green Leaf Cafe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indirect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whitechapel Rd, London</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hot beverages, Coffee, Paan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$5 - $20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cafegreenleaf.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">International</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesmerizing taste &amp; aroma</t>
   </si>
 </sst>
 </file>
@@ -350,7 +991,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -424,6 +1065,12 @@
       <name val="Google Sans"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Google Sans"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="14">
@@ -540,104 +1187,108 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -721,339 +1372,339 @@
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="O1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topRight" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="10" style="0" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="10" style="1" width="35.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="J2" s="4" t="s">
+      <c r="A2" s="4"/>
+      <c r="J2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="J3" s="5" t="s">
+      <c r="A3" s="4"/>
+      <c r="J3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="6" t="s">
+      <c r="K3" s="6"/>
+      <c r="L3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="7" t="s">
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="8"/>
+      <c r="R3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="P5" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="22" t="s">
+      <c r="K5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="23" t="s">
+      <c r="L5" s="21" t="s">
         <v>34</v>
       </c>
+      <c r="M5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="24" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="15" t="s">
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="17" t="s">
+      <c r="C6" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="P6" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q6" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="23" t="s">
-        <v>34</v>
+      <c r="I6" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="R6" s="24" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="15" t="s">
+    <row r="7" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="N7" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="P7" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q7" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" s="23" t="s">
-        <v>34</v>
+      <c r="H7" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="R7" s="24" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="L8" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="P8" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q8" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="23" t="s">
-        <v>34</v>
+    <row r="8" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="P8" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q8" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="R8" s="24" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>